<commit_message>
some clean-code-rules in table
</commit_message>
<xml_diff>
--- a/files/sq_rules.xlsx
+++ b/files/sq_rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1958" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="589">
   <si>
     <t>blocker</t>
   </si>
@@ -1708,9 +1708,6 @@
     <t>Rule</t>
   </si>
   <si>
-    <t>SonarQube-Tags / Comments</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -1733,6 +1730,57 @@
   </si>
   <si>
     <t>J-Style</t>
+  </si>
+  <si>
+    <t>maximal 3</t>
+  </si>
+  <si>
+    <t>SonarQube-Tags</t>
+  </si>
+  <si>
+    <t>Clean-Code-Comment</t>
+  </si>
+  <si>
+    <t>"Output-Argumente"</t>
+  </si>
+  <si>
+    <t>keine Flag-Argumente (Boolean Parameter)</t>
+  </si>
+  <si>
+    <t>NONAUTOMATIC</t>
+  </si>
+  <si>
+    <t>Keine ungeeigneten Informationen in Kommentaren</t>
+  </si>
+  <si>
+    <t>Keine überholten Kommentare</t>
+  </si>
+  <si>
+    <t>Keine redundanten Kommentare</t>
+  </si>
+  <si>
+    <t>Keine schlecht geschriebenen Kommentare</t>
+  </si>
+  <si>
+    <t>Ein Build sollte nur einen Schritt erfordern</t>
+  </si>
+  <si>
+    <t>Testausführung sollte nur einen Schritt erfordern</t>
+  </si>
+  <si>
+    <t>Nur eine Sprache je Quelldatei</t>
+  </si>
+  <si>
+    <t>Offensichtlich erwartetes Verhalten implementieren</t>
+  </si>
+  <si>
+    <t>Alle Grenzbedingungen, Sonderfälle, Eigenheiten und Ausnahmen durch Tests abdecken</t>
+  </si>
+  <si>
+    <t>Keine Sicherungen / Tests übergehen</t>
+  </si>
+  <si>
+    <t>Auf der richtigen Abstraktionsebene Codieren</t>
   </si>
 </sst>
 </file>
@@ -2562,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L378"/>
+  <dimension ref="A1:M390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="D358" workbookViewId="0">
+      <selection activeCell="D358" sqref="D358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2580,10 +2628,11 @@
     <col min="9" max="9" width="8.5546875" customWidth="1"/>
     <col min="10" max="10" width="9.44140625" customWidth="1"/>
     <col min="11" max="11" width="7.21875" customWidth="1"/>
-    <col min="12" max="12" width="54.5546875" customWidth="1"/>
+    <col min="12" max="12" width="51" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>562</v>
       </c>
@@ -2597,31 +2646,34 @@
         <v>563</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>572</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>573</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2632,13 +2684,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2649,13 +2701,13 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2666,13 +2718,13 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2683,13 +2735,13 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2700,13 +2752,13 @@
         <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2717,13 +2769,13 @@
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2734,13 +2786,13 @@
         <v>89</v>
       </c>
       <c r="E8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2751,13 +2803,13 @@
         <v>94</v>
       </c>
       <c r="E9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2768,13 +2820,13 @@
         <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2785,13 +2837,13 @@
         <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2802,13 +2854,13 @@
         <v>138</v>
       </c>
       <c r="E12" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2819,13 +2871,13 @@
         <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2836,13 +2888,13 @@
         <v>222</v>
       </c>
       <c r="E14" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2853,13 +2905,13 @@
         <v>232</v>
       </c>
       <c r="E15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2870,7 +2922,7 @@
         <v>308</v>
       </c>
       <c r="E16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L16" t="s">
         <v>309</v>
@@ -2887,7 +2939,7 @@
         <v>338</v>
       </c>
       <c r="E17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L17" t="s">
         <v>17</v>
@@ -2904,7 +2956,7 @@
         <v>350</v>
       </c>
       <c r="E18" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L18" t="s">
         <v>2</v>
@@ -2921,7 +2973,7 @@
         <v>384</v>
       </c>
       <c r="E19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L19" t="s">
         <v>385</v>
@@ -2938,7 +2990,7 @@
         <v>391</v>
       </c>
       <c r="E20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L20" t="s">
         <v>70</v>
@@ -2955,7 +3007,7 @@
         <v>413</v>
       </c>
       <c r="E21" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L21" t="s">
         <v>8</v>
@@ -2972,7 +3024,7 @@
         <v>416</v>
       </c>
       <c r="E22" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L22" t="s">
         <v>417</v>
@@ -2989,7 +3041,7 @@
         <v>432</v>
       </c>
       <c r="E23" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L23" t="s">
         <v>8</v>
@@ -3006,7 +3058,7 @@
         <v>455</v>
       </c>
       <c r="E24" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L24" t="s">
         <v>39</v>
@@ -3023,7 +3075,7 @@
         <v>457</v>
       </c>
       <c r="E25" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L25" t="s">
         <v>78</v>
@@ -3040,7 +3092,7 @@
         <v>475</v>
       </c>
       <c r="E26" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L26" t="s">
         <v>17</v>
@@ -3057,7 +3109,7 @@
         <v>479</v>
       </c>
       <c r="E27" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L27" t="s">
         <v>286</v>
@@ -3074,7 +3126,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L28" t="s">
         <v>8</v>
@@ -3091,7 +3143,7 @@
         <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L29" t="s">
         <v>17</v>
@@ -3108,7 +3160,7 @@
         <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L30" t="s">
         <v>8</v>
@@ -3125,7 +3177,7 @@
         <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L31" t="s">
         <v>8</v>
@@ -3142,7 +3194,7 @@
         <v>27</v>
       </c>
       <c r="E32" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L32" t="s">
         <v>28</v>
@@ -3159,7 +3211,7 @@
         <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L33" t="s">
         <v>36</v>
@@ -3176,7 +3228,7 @@
         <v>37</v>
       </c>
       <c r="E34" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L34" t="s">
         <v>17</v>
@@ -3196,7 +3248,7 @@
         <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L35" t="s">
         <v>8</v>
@@ -3213,7 +3265,7 @@
         <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L36" t="s">
         <v>43</v>
@@ -3230,7 +3282,7 @@
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L37" t="s">
         <v>8</v>
@@ -3247,7 +3299,7 @@
         <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L38" t="s">
         <v>46</v>
@@ -3264,7 +3316,7 @@
         <v>56</v>
       </c>
       <c r="E39" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L39" t="s">
         <v>8</v>
@@ -3281,7 +3333,7 @@
         <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L40" t="s">
         <v>58</v>
@@ -3298,7 +3350,7 @@
         <v>63</v>
       </c>
       <c r="E41" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L41" t="s">
         <v>64</v>
@@ -3315,7 +3367,7 @@
         <v>73</v>
       </c>
       <c r="E42" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L42" t="s">
         <v>74</v>
@@ -3332,7 +3384,7 @@
         <v>77</v>
       </c>
       <c r="E43" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L43" t="s">
         <v>78</v>
@@ -3352,7 +3404,7 @@
         <v>83</v>
       </c>
       <c r="E44" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L44" t="s">
         <v>84</v>
@@ -3369,7 +3421,7 @@
         <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L45" t="s">
         <v>78</v>
@@ -3386,7 +3438,7 @@
         <v>93</v>
       </c>
       <c r="E46" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L46" t="s">
         <v>86</v>
@@ -3403,7 +3455,7 @@
         <v>105</v>
       </c>
       <c r="E47" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L47" t="s">
         <v>106</v>
@@ -3420,7 +3472,7 @@
         <v>107</v>
       </c>
       <c r="E48" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L48" t="s">
         <v>108</v>
@@ -3440,7 +3492,7 @@
         <v>109</v>
       </c>
       <c r="E49" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L49" t="s">
         <v>110</v>
@@ -3457,7 +3509,7 @@
         <v>125</v>
       </c>
       <c r="E50" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L50" t="s">
         <v>8</v>
@@ -3474,7 +3526,7 @@
         <v>128</v>
       </c>
       <c r="E51" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L51" t="s">
         <v>129</v>
@@ -3491,7 +3543,7 @@
         <v>133</v>
       </c>
       <c r="E52" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L52" t="s">
         <v>134</v>
@@ -3508,7 +3560,7 @@
         <v>135</v>
       </c>
       <c r="E53" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L53" t="s">
         <v>2</v>
@@ -3525,7 +3577,7 @@
         <v>157</v>
       </c>
       <c r="E54" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L54" t="s">
         <v>158</v>
@@ -3542,7 +3594,7 @@
         <v>184</v>
       </c>
       <c r="E55" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L55" t="s">
         <v>185</v>
@@ -3559,7 +3611,7 @@
         <v>188</v>
       </c>
       <c r="E56" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L56" t="s">
         <v>189</v>
@@ -3576,7 +3628,7 @@
         <v>192</v>
       </c>
       <c r="E57" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L57" t="s">
         <v>8</v>
@@ -3593,7 +3645,7 @@
         <v>202</v>
       </c>
       <c r="E58" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L58" t="s">
         <v>8</v>
@@ -3610,7 +3662,7 @@
         <v>208</v>
       </c>
       <c r="E59" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L59" t="s">
         <v>209</v>
@@ -3627,7 +3679,7 @@
         <v>220</v>
       </c>
       <c r="E60" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L60" t="s">
         <v>221</v>
@@ -3644,7 +3696,7 @@
         <v>223</v>
       </c>
       <c r="E61" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L61" t="s">
         <v>224</v>
@@ -3661,7 +3713,7 @@
         <v>225</v>
       </c>
       <c r="E62" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L62" t="s">
         <v>226</v>
@@ -3678,7 +3730,7 @@
         <v>227</v>
       </c>
       <c r="E63" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L63" t="s">
         <v>17</v>
@@ -3695,7 +3747,7 @@
         <v>243</v>
       </c>
       <c r="E64" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L64" t="s">
         <v>8</v>
@@ -3712,7 +3764,7 @@
         <v>257</v>
       </c>
       <c r="E65" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L65" t="s">
         <v>258</v>
@@ -3729,7 +3781,7 @@
         <v>270</v>
       </c>
       <c r="E66" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L66" t="s">
         <v>271</v>
@@ -3749,7 +3801,7 @@
         <v>281</v>
       </c>
       <c r="E67" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L67" t="s">
         <v>282</v>
@@ -3766,7 +3818,7 @@
         <v>285</v>
       </c>
       <c r="E68" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L68" t="s">
         <v>286</v>
@@ -3783,7 +3835,7 @@
         <v>288</v>
       </c>
       <c r="E69" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L69" t="s">
         <v>78</v>
@@ -3800,7 +3852,7 @@
         <v>290</v>
       </c>
       <c r="E70" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L70" t="s">
         <v>58</v>
@@ -3817,7 +3869,7 @@
         <v>291</v>
       </c>
       <c r="E71" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L71" t="s">
         <v>17</v>
@@ -3834,7 +3886,7 @@
         <v>292</v>
       </c>
       <c r="E72" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L72" t="s">
         <v>2</v>
@@ -3851,7 +3903,7 @@
         <v>293</v>
       </c>
       <c r="E73" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L73" t="s">
         <v>17</v>
@@ -3868,7 +3920,7 @@
         <v>294</v>
       </c>
       <c r="E74" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L74" t="s">
         <v>8</v>
@@ -3885,7 +3937,7 @@
         <v>301</v>
       </c>
       <c r="E75" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L75" t="s">
         <v>2</v>
@@ -3902,7 +3954,7 @@
         <v>303</v>
       </c>
       <c r="E76" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L76" t="s">
         <v>17</v>
@@ -3919,7 +3971,7 @@
         <v>304</v>
       </c>
       <c r="E77" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L77" t="s">
         <v>8</v>
@@ -3936,7 +3988,7 @@
         <v>305</v>
       </c>
       <c r="E78" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L78" t="s">
         <v>306</v>
@@ -3953,7 +4005,7 @@
         <v>312</v>
       </c>
       <c r="E79" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L79" t="s">
         <v>158</v>
@@ -3970,7 +4022,7 @@
         <v>313</v>
       </c>
       <c r="E80" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L80" t="s">
         <v>158</v>
@@ -3987,7 +4039,7 @@
         <v>316</v>
       </c>
       <c r="E81" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L81" t="s">
         <v>158</v>
@@ -4004,7 +4056,7 @@
         <v>321</v>
       </c>
       <c r="E82" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L82" t="s">
         <v>2</v>
@@ -4021,7 +4073,7 @@
         <v>333</v>
       </c>
       <c r="E83" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L83" t="s">
         <v>64</v>
@@ -4038,7 +4090,7 @@
         <v>337</v>
       </c>
       <c r="E84" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L84" t="s">
         <v>8</v>
@@ -4058,7 +4110,7 @@
         <v>342</v>
       </c>
       <c r="E85" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L85" t="s">
         <v>343</v>
@@ -4075,7 +4127,7 @@
         <v>344</v>
       </c>
       <c r="E86" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L86" t="s">
         <v>17</v>
@@ -4092,7 +4144,7 @@
         <v>345</v>
       </c>
       <c r="E87" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L87" t="s">
         <v>346</v>
@@ -4109,7 +4161,7 @@
         <v>355</v>
       </c>
       <c r="E88" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L88" t="s">
         <v>356</v>
@@ -4126,7 +4178,7 @@
         <v>365</v>
       </c>
       <c r="E89" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L89" t="s">
         <v>39</v>
@@ -4143,7 +4195,7 @@
         <v>369</v>
       </c>
       <c r="E90" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L90" t="s">
         <v>370</v>
@@ -4160,7 +4212,7 @@
         <v>371</v>
       </c>
       <c r="E91" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L91" t="s">
         <v>370</v>
@@ -4177,7 +4229,7 @@
         <v>372</v>
       </c>
       <c r="E92" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L92" t="s">
         <v>8</v>
@@ -4194,7 +4246,7 @@
         <v>373</v>
       </c>
       <c r="E93" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L93" t="s">
         <v>374</v>
@@ -4211,7 +4263,7 @@
         <v>379</v>
       </c>
       <c r="E94" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L94" t="s">
         <v>108</v>
@@ -4228,7 +4280,7 @@
         <v>380</v>
       </c>
       <c r="E95" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L95" t="s">
         <v>381</v>
@@ -4245,7 +4297,7 @@
         <v>382</v>
       </c>
       <c r="E96" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L96" t="s">
         <v>129</v>
@@ -4262,7 +4314,7 @@
         <v>383</v>
       </c>
       <c r="E97" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L97" t="s">
         <v>2</v>
@@ -4282,7 +4334,7 @@
         <v>389</v>
       </c>
       <c r="E98" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L98" t="s">
         <v>84</v>
@@ -4299,7 +4351,7 @@
         <v>402</v>
       </c>
       <c r="E99" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L99" t="s">
         <v>403</v>
@@ -4316,7 +4368,7 @@
         <v>404</v>
       </c>
       <c r="E100" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L100" t="s">
         <v>405</v>
@@ -4333,7 +4385,7 @@
         <v>410</v>
       </c>
       <c r="E101" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L101" t="s">
         <v>17</v>
@@ -4350,7 +4402,7 @@
         <v>414</v>
       </c>
       <c r="E102" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L102" t="s">
         <v>415</v>
@@ -4367,7 +4419,7 @@
         <v>419</v>
       </c>
       <c r="E103" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L103" t="s">
         <v>420</v>
@@ -4384,7 +4436,7 @@
         <v>421</v>
       </c>
       <c r="E104" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L104" t="s">
         <v>422</v>
@@ -4401,7 +4453,7 @@
         <v>425</v>
       </c>
       <c r="E105" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L105" t="s">
         <v>426</v>
@@ -4418,7 +4470,7 @@
         <v>427</v>
       </c>
       <c r="E106" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L106" t="s">
         <v>428</v>
@@ -4435,7 +4487,7 @@
         <v>430</v>
       </c>
       <c r="E107" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L107" t="s">
         <v>70</v>
@@ -4452,7 +4504,7 @@
         <v>431</v>
       </c>
       <c r="E108" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L108" t="s">
         <v>17</v>
@@ -4469,7 +4521,7 @@
         <v>434</v>
       </c>
       <c r="E109" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L109" t="s">
         <v>435</v>
@@ -4489,7 +4541,7 @@
         <v>449</v>
       </c>
       <c r="E110" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L110" t="s">
         <v>450</v>
@@ -4506,7 +4558,7 @@
         <v>452</v>
       </c>
       <c r="E111" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L111" t="s">
         <v>453</v>
@@ -4523,7 +4575,7 @@
         <v>463</v>
       </c>
       <c r="E112" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L112" t="s">
         <v>311</v>
@@ -4543,7 +4595,7 @@
         <v>467</v>
       </c>
       <c r="E113" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L113" t="s">
         <v>84</v>
@@ -4560,7 +4612,7 @@
         <v>470</v>
       </c>
       <c r="E114" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L114" t="s">
         <v>381</v>
@@ -4577,7 +4629,7 @@
         <v>471</v>
       </c>
       <c r="E115" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L115" t="s">
         <v>86</v>
@@ -4594,7 +4646,7 @@
         <v>476</v>
       </c>
       <c r="E116" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L116" t="s">
         <v>477</v>
@@ -4614,7 +4666,7 @@
         <v>480</v>
       </c>
       <c r="E117" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L117" t="s">
         <v>74</v>
@@ -4631,7 +4683,7 @@
         <v>488</v>
       </c>
       <c r="E118" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L118" t="s">
         <v>489</v>
@@ -4648,7 +4700,7 @@
         <v>503</v>
       </c>
       <c r="E119" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L119" t="s">
         <v>504</v>
@@ -4665,7 +4717,7 @@
         <v>505</v>
       </c>
       <c r="E120" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L120" t="s">
         <v>506</v>
@@ -4682,7 +4734,7 @@
         <v>507</v>
       </c>
       <c r="E121" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L121" t="s">
         <v>508</v>
@@ -4699,7 +4751,7 @@
         <v>509</v>
       </c>
       <c r="E122" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L122" t="s">
         <v>8</v>
@@ -4716,7 +4768,7 @@
         <v>511</v>
       </c>
       <c r="E123" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L123" t="s">
         <v>17</v>
@@ -4733,7 +4785,7 @@
         <v>512</v>
       </c>
       <c r="E124" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L124" t="s">
         <v>513</v>
@@ -4750,7 +4802,7 @@
         <v>514</v>
       </c>
       <c r="E125" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L125" t="s">
         <v>515</v>
@@ -4767,7 +4819,7 @@
         <v>10</v>
       </c>
       <c r="E126" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L126" t="s">
         <v>11</v>
@@ -4784,7 +4836,7 @@
         <v>12</v>
       </c>
       <c r="E127" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L127" t="s">
         <v>13</v>
@@ -4801,7 +4853,7 @@
         <v>14</v>
       </c>
       <c r="E128" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L128" t="s">
         <v>15</v>
@@ -4818,7 +4870,7 @@
         <v>21</v>
       </c>
       <c r="E129" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L129" t="s">
         <v>22</v>
@@ -4835,7 +4887,7 @@
         <v>24</v>
       </c>
       <c r="E130" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L130" t="s">
         <v>25</v>
@@ -4852,7 +4904,7 @@
         <v>29</v>
       </c>
       <c r="E131" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L131" t="s">
         <v>30</v>
@@ -4869,7 +4921,7 @@
         <v>31</v>
       </c>
       <c r="E132" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L132" t="s">
         <v>32</v>
@@ -4886,7 +4938,7 @@
         <v>34</v>
       </c>
       <c r="E133" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L133" t="s">
         <v>32</v>
@@ -4903,7 +4955,7 @@
         <v>47</v>
       </c>
       <c r="E134" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L134" t="s">
         <v>48</v>
@@ -4920,7 +4972,7 @@
         <v>49</v>
       </c>
       <c r="E135" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L135" t="s">
         <v>50</v>
@@ -4937,7 +4989,7 @@
         <v>51</v>
       </c>
       <c r="E136" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L136" t="s">
         <v>52</v>
@@ -4954,7 +5006,7 @@
         <v>53</v>
       </c>
       <c r="E137" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L137" t="s">
         <v>22</v>
@@ -4971,7 +5023,7 @@
         <v>54</v>
       </c>
       <c r="E138" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L138" t="s">
         <v>55</v>
@@ -4988,7 +5040,7 @@
         <v>59</v>
       </c>
       <c r="E139" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L139" t="s">
         <v>22</v>
@@ -5005,7 +5057,7 @@
         <v>60</v>
       </c>
       <c r="E140" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L140" t="s">
         <v>48</v>
@@ -5022,7 +5074,7 @@
         <v>61</v>
       </c>
       <c r="E141" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L141" t="s">
         <v>62</v>
@@ -5042,7 +5094,7 @@
         <v>66</v>
       </c>
       <c r="E142" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L142" t="s">
         <v>25</v>
@@ -5059,7 +5111,7 @@
         <v>71</v>
       </c>
       <c r="E143" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L143" t="s">
         <v>72</v>
@@ -5076,7 +5128,7 @@
         <v>76</v>
       </c>
       <c r="E144" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L144" t="s">
         <v>11</v>
@@ -5093,7 +5145,7 @@
         <v>79</v>
       </c>
       <c r="E145" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L145" t="s">
         <v>80</v>
@@ -5110,7 +5162,7 @@
         <v>81</v>
       </c>
       <c r="E146" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L146" t="s">
         <v>82</v>
@@ -5127,7 +5179,7 @@
         <v>85</v>
       </c>
       <c r="E147" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L147" t="s">
         <v>86</v>
@@ -5147,7 +5199,7 @@
         <v>88</v>
       </c>
       <c r="E148" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L148" t="s">
         <v>22</v>
@@ -5164,7 +5216,7 @@
         <v>91</v>
       </c>
       <c r="E149" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L149" t="s">
         <v>48</v>
@@ -5184,7 +5236,7 @@
         <v>95</v>
       </c>
       <c r="E150" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L150" t="s">
         <v>48</v>
@@ -5201,7 +5253,7 @@
         <v>96</v>
       </c>
       <c r="E151" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L151" t="s">
         <v>82</v>
@@ -5218,7 +5270,7 @@
         <v>97</v>
       </c>
       <c r="E152" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L152" t="s">
         <v>98</v>
@@ -5235,7 +5287,7 @@
         <v>102</v>
       </c>
       <c r="E153" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L153" t="s">
         <v>103</v>
@@ -5252,7 +5304,7 @@
         <v>104</v>
       </c>
       <c r="E154" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L154" t="s">
         <v>103</v>
@@ -5269,7 +5321,7 @@
         <v>111</v>
       </c>
       <c r="E155" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L155" t="s">
         <v>82</v>
@@ -5286,7 +5338,7 @@
         <v>112</v>
       </c>
       <c r="E156" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L156" t="s">
         <v>82</v>
@@ -5303,7 +5355,7 @@
         <v>113</v>
       </c>
       <c r="E157" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L157" t="s">
         <v>114</v>
@@ -5320,7 +5372,7 @@
         <v>115</v>
       </c>
       <c r="E158" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L158" t="s">
         <v>116</v>
@@ -5337,7 +5389,7 @@
         <v>119</v>
       </c>
       <c r="E159" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L159" t="s">
         <v>120</v>
@@ -5354,7 +5406,7 @@
         <v>121</v>
       </c>
       <c r="E160" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L160" t="s">
         <v>114</v>
@@ -5374,7 +5426,7 @@
         <v>122</v>
       </c>
       <c r="E161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L161" t="s">
         <v>11</v>
@@ -5391,7 +5443,7 @@
         <v>123</v>
       </c>
       <c r="E162" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L162" t="s">
         <v>124</v>
@@ -5411,7 +5463,7 @@
         <v>132</v>
       </c>
       <c r="E163" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L163" t="s">
         <v>32</v>
@@ -5428,7 +5480,7 @@
         <v>136</v>
       </c>
       <c r="E164" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L164" t="s">
         <v>137</v>
@@ -5445,7 +5497,7 @@
         <v>143</v>
       </c>
       <c r="E165" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L165" t="s">
         <v>114</v>
@@ -5462,7 +5514,7 @@
         <v>145</v>
       </c>
       <c r="E166" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L166" t="s">
         <v>137</v>
@@ -5479,7 +5531,7 @@
         <v>146</v>
       </c>
       <c r="E167" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L167" t="s">
         <v>48</v>
@@ -5496,7 +5548,7 @@
         <v>151</v>
       </c>
       <c r="E168" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L168" t="s">
         <v>137</v>
@@ -5516,7 +5568,7 @@
         <v>152</v>
       </c>
       <c r="E169" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L169" t="s">
         <v>137</v>
@@ -5536,7 +5588,7 @@
         <v>159</v>
       </c>
       <c r="E170" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L170" t="s">
         <v>160</v>
@@ -5553,7 +5605,7 @@
         <v>165</v>
       </c>
       <c r="E171" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L171" t="s">
         <v>140</v>
@@ -5570,7 +5622,7 @@
         <v>166</v>
       </c>
       <c r="E172" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L172" t="s">
         <v>11</v>
@@ -5587,7 +5639,7 @@
         <v>167</v>
       </c>
       <c r="E173" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L173" t="s">
         <v>140</v>
@@ -5604,7 +5656,7 @@
         <v>168</v>
       </c>
       <c r="E174" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L174" t="s">
         <v>140</v>
@@ -5621,7 +5673,7 @@
         <v>169</v>
       </c>
       <c r="E175" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L175" t="s">
         <v>68</v>
@@ -5638,7 +5690,7 @@
         <v>170</v>
       </c>
       <c r="E176" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L176" t="s">
         <v>48</v>
@@ -5655,7 +5707,7 @@
         <v>171</v>
       </c>
       <c r="E177" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L177" t="s">
         <v>82</v>
@@ -5672,7 +5724,7 @@
         <v>173</v>
       </c>
       <c r="E178" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L178" t="s">
         <v>82</v>
@@ -5689,7 +5741,7 @@
         <v>174</v>
       </c>
       <c r="E179" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L179" t="s">
         <v>175</v>
@@ -5709,7 +5761,7 @@
         <v>176</v>
       </c>
       <c r="E180" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L180" t="s">
         <v>82</v>
@@ -5729,7 +5781,7 @@
         <v>177</v>
       </c>
       <c r="E181" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L181" t="s">
         <v>178</v>
@@ -5746,7 +5798,7 @@
         <v>179</v>
       </c>
       <c r="E182" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L182" t="s">
         <v>124</v>
@@ -5763,7 +5815,7 @@
         <v>180</v>
       </c>
       <c r="E183" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L183" t="s">
         <v>181</v>
@@ -5780,7 +5832,7 @@
         <v>182</v>
       </c>
       <c r="E184" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L184" t="s">
         <v>183</v>
@@ -5800,7 +5852,7 @@
         <v>186</v>
       </c>
       <c r="E185" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L185" t="s">
         <v>114</v>
@@ -5817,7 +5869,7 @@
         <v>187</v>
       </c>
       <c r="E186" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L186" t="s">
         <v>140</v>
@@ -5834,7 +5886,7 @@
         <v>190</v>
       </c>
       <c r="E187" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L187" t="s">
         <v>114</v>
@@ -5851,7 +5903,7 @@
         <v>191</v>
       </c>
       <c r="E188" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L188" t="s">
         <v>114</v>
@@ -5871,7 +5923,7 @@
         <v>193</v>
       </c>
       <c r="E189" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L189" t="s">
         <v>194</v>
@@ -5891,7 +5943,7 @@
         <v>195</v>
       </c>
       <c r="E190" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L190" t="s">
         <v>140</v>
@@ -5908,7 +5960,7 @@
         <v>196</v>
       </c>
       <c r="E191" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L191" t="s">
         <v>197</v>
@@ -5925,7 +5977,7 @@
         <v>200</v>
       </c>
       <c r="E192" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L192" t="s">
         <v>140</v>
@@ -5942,7 +5994,7 @@
         <v>201</v>
       </c>
       <c r="E193" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L193" t="s">
         <v>140</v>
@@ -5959,7 +6011,7 @@
         <v>203</v>
       </c>
       <c r="E194" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L194" t="s">
         <v>204</v>
@@ -5976,7 +6028,7 @@
         <v>206</v>
       </c>
       <c r="E195" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L195" t="s">
         <v>207</v>
@@ -5996,7 +6048,7 @@
         <v>212</v>
       </c>
       <c r="E196" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L196" t="s">
         <v>213</v>
@@ -6013,7 +6065,7 @@
         <v>214</v>
       </c>
       <c r="E197" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L197" t="s">
         <v>32</v>
@@ -6030,7 +6082,7 @@
         <v>215</v>
       </c>
       <c r="E198" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L198" t="s">
         <v>216</v>
@@ -6047,7 +6099,7 @@
         <v>217</v>
       </c>
       <c r="E199" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L199" t="s">
         <v>114</v>
@@ -6067,7 +6119,7 @@
         <v>218</v>
       </c>
       <c r="E200" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L200" t="s">
         <v>219</v>
@@ -6084,7 +6136,7 @@
         <v>228</v>
       </c>
       <c r="E201" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L201" t="s">
         <v>197</v>
@@ -6104,7 +6156,7 @@
         <v>229</v>
       </c>
       <c r="E202" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L202" t="s">
         <v>230</v>
@@ -6121,7 +6173,7 @@
         <v>231</v>
       </c>
       <c r="E203" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L203" t="s">
         <v>11</v>
@@ -6138,7 +6190,7 @@
         <v>233</v>
       </c>
       <c r="E204" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L204" t="s">
         <v>234</v>
@@ -6158,7 +6210,7 @@
         <v>235</v>
       </c>
       <c r="E205" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L205" t="s">
         <v>236</v>
@@ -6178,7 +6230,7 @@
         <v>237</v>
       </c>
       <c r="E206" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L206" t="s">
         <v>238</v>
@@ -6195,7 +6247,7 @@
         <v>241</v>
       </c>
       <c r="E207" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L207" t="s">
         <v>242</v>
@@ -6212,7 +6264,7 @@
         <v>244</v>
       </c>
       <c r="E208" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L208" t="s">
         <v>82</v>
@@ -6232,7 +6284,7 @@
         <v>245</v>
       </c>
       <c r="E209" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L209" t="s">
         <v>246</v>
@@ -6249,7 +6301,7 @@
         <v>249</v>
       </c>
       <c r="E210" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L210" t="s">
         <v>240</v>
@@ -6266,7 +6318,7 @@
         <v>250</v>
       </c>
       <c r="E211" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L211" t="s">
         <v>160</v>
@@ -6283,7 +6335,7 @@
         <v>251</v>
       </c>
       <c r="E212" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L212" t="s">
         <v>48</v>
@@ -6300,7 +6352,7 @@
         <v>252</v>
       </c>
       <c r="E213" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L213" t="s">
         <v>68</v>
@@ -6317,7 +6369,7 @@
         <v>253</v>
       </c>
       <c r="E214" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L214" t="s">
         <v>254</v>
@@ -6334,7 +6386,7 @@
         <v>255</v>
       </c>
       <c r="E215" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L215" t="s">
         <v>256</v>
@@ -6351,7 +6403,7 @@
         <v>259</v>
       </c>
       <c r="E216" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L216" t="s">
         <v>254</v>
@@ -6368,7 +6420,7 @@
         <v>260</v>
       </c>
       <c r="E217" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L217" t="s">
         <v>261</v>
@@ -6385,7 +6437,7 @@
         <v>262</v>
       </c>
       <c r="E218" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L218" t="s">
         <v>263</v>
@@ -6402,7 +6454,7 @@
         <v>264</v>
       </c>
       <c r="E219" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L219" t="s">
         <v>114</v>
@@ -6419,7 +6471,7 @@
         <v>266</v>
       </c>
       <c r="E220" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L220" t="s">
         <v>8</v>
@@ -6439,7 +6491,7 @@
         <v>268</v>
       </c>
       <c r="E221" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L221" t="s">
         <v>269</v>
@@ -6456,7 +6508,7 @@
         <v>277</v>
       </c>
       <c r="E222" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L222" t="s">
         <v>114</v>
@@ -6476,7 +6528,7 @@
         <v>278</v>
       </c>
       <c r="E223" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L223" t="s">
         <v>279</v>
@@ -6493,7 +6545,7 @@
         <v>280</v>
       </c>
       <c r="E224" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L224" t="s">
         <v>114</v>
@@ -6510,7 +6562,7 @@
         <v>284</v>
       </c>
       <c r="E225" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L225" t="s">
         <v>204</v>
@@ -6530,7 +6582,7 @@
         <v>287</v>
       </c>
       <c r="E226" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L226" t="s">
         <v>82</v>
@@ -6547,7 +6599,7 @@
         <v>295</v>
       </c>
       <c r="E227" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L227" t="s">
         <v>296</v>
@@ -6564,7 +6616,7 @@
         <v>297</v>
       </c>
       <c r="E228" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L228" t="s">
         <v>197</v>
@@ -6581,7 +6633,7 @@
         <v>298</v>
       </c>
       <c r="E229" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L229" t="s">
         <v>82</v>
@@ -6598,7 +6650,7 @@
         <v>299</v>
       </c>
       <c r="E230" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L230" t="s">
         <v>114</v>
@@ -6615,7 +6667,7 @@
         <v>300</v>
       </c>
       <c r="E231" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L231" t="s">
         <v>32</v>
@@ -6632,7 +6684,7 @@
         <v>307</v>
       </c>
       <c r="E232" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L232" t="s">
         <v>22</v>
@@ -6649,7 +6701,7 @@
         <v>310</v>
       </c>
       <c r="E233" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L233" t="s">
         <v>311</v>
@@ -6666,7 +6718,7 @@
         <v>314</v>
       </c>
       <c r="E234" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L234" t="s">
         <v>315</v>
@@ -6683,7 +6735,7 @@
         <v>317</v>
       </c>
       <c r="E235" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L235" t="s">
         <v>48</v>
@@ -6703,7 +6755,7 @@
         <v>318</v>
       </c>
       <c r="E236" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L236" t="s">
         <v>137</v>
@@ -6720,7 +6772,7 @@
         <v>320</v>
       </c>
       <c r="E237" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L237" t="s">
         <v>137</v>
@@ -6737,7 +6789,7 @@
         <v>322</v>
       </c>
       <c r="E238" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L238" t="s">
         <v>116</v>
@@ -6754,7 +6806,7 @@
         <v>323</v>
       </c>
       <c r="E239" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L239" t="s">
         <v>11</v>
@@ -6771,13 +6823,13 @@
         <v>325</v>
       </c>
       <c r="E240" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L240" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>9</v>
       </c>
@@ -6788,13 +6840,13 @@
         <v>331</v>
       </c>
       <c r="E241" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L241" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>9</v>
       </c>
@@ -6805,13 +6857,13 @@
         <v>332</v>
       </c>
       <c r="E242" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L242" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -6822,13 +6874,13 @@
         <v>339</v>
       </c>
       <c r="E243" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L243" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>9</v>
       </c>
@@ -6839,13 +6891,13 @@
         <v>341</v>
       </c>
       <c r="E244" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L244" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>9</v>
       </c>
@@ -6859,13 +6911,13 @@
         <v>348</v>
       </c>
       <c r="E245" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L245" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>9</v>
       </c>
@@ -6879,13 +6931,19 @@
         <v>349</v>
       </c>
       <c r="E246" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="G246" t="s">
+        <v>564</v>
       </c>
       <c r="L246" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M246" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>9</v>
       </c>
@@ -6899,13 +6957,13 @@
         <v>351</v>
       </c>
       <c r="E247" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L247" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>9</v>
       </c>
@@ -6919,13 +6977,13 @@
         <v>352</v>
       </c>
       <c r="E248" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L248" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>9</v>
       </c>
@@ -6936,13 +6994,13 @@
         <v>353</v>
       </c>
       <c r="E249" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L249" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>9</v>
       </c>
@@ -6953,13 +7011,13 @@
         <v>354</v>
       </c>
       <c r="E250" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L250" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>9</v>
       </c>
@@ -6973,13 +7031,13 @@
         <v>357</v>
       </c>
       <c r="E251" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L251" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>9</v>
       </c>
@@ -6990,13 +7048,13 @@
         <v>358</v>
       </c>
       <c r="E252" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L252" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>9</v>
       </c>
@@ -7007,13 +7065,19 @@
         <v>359</v>
       </c>
       <c r="E253" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="G253" t="s">
+        <v>564</v>
       </c>
       <c r="L253" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M253" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>9</v>
       </c>
@@ -7027,13 +7091,13 @@
         <v>360</v>
       </c>
       <c r="E254" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L254" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>9</v>
       </c>
@@ -7047,13 +7111,13 @@
         <v>361</v>
       </c>
       <c r="E255" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L255" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>9</v>
       </c>
@@ -7064,7 +7128,7 @@
         <v>364</v>
       </c>
       <c r="E256" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L256" t="s">
         <v>15</v>
@@ -7081,7 +7145,7 @@
         <v>366</v>
       </c>
       <c r="E257" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L257" t="s">
         <v>32</v>
@@ -7098,7 +7162,7 @@
         <v>375</v>
       </c>
       <c r="E258" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L258" t="s">
         <v>140</v>
@@ -7115,7 +7179,7 @@
         <v>376</v>
       </c>
       <c r="E259" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L259" t="s">
         <v>22</v>
@@ -7132,7 +7196,7 @@
         <v>377</v>
       </c>
       <c r="E260" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L260" t="s">
         <v>11</v>
@@ -7152,7 +7216,7 @@
         <v>378</v>
       </c>
       <c r="E261" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L261" t="s">
         <v>82</v>
@@ -7172,7 +7236,7 @@
         <v>386</v>
       </c>
       <c r="E262" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L262" t="s">
         <v>82</v>
@@ -7189,7 +7253,7 @@
         <v>387</v>
       </c>
       <c r="E263" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L263" t="s">
         <v>194</v>
@@ -7206,7 +7270,7 @@
         <v>388</v>
       </c>
       <c r="E264" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L264" t="s">
         <v>32</v>
@@ -7223,7 +7287,7 @@
         <v>390</v>
       </c>
       <c r="E265" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L265" t="s">
         <v>219</v>
@@ -7243,7 +7307,7 @@
         <v>392</v>
       </c>
       <c r="E266" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L266" t="s">
         <v>82</v>
@@ -7260,7 +7324,7 @@
         <v>394</v>
       </c>
       <c r="E267" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L267" t="s">
         <v>82</v>
@@ -7277,7 +7341,7 @@
         <v>398</v>
       </c>
       <c r="E268" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L268" t="s">
         <v>32</v>
@@ -7294,7 +7358,7 @@
         <v>400</v>
       </c>
       <c r="E269" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L269" t="s">
         <v>140</v>
@@ -7311,7 +7375,7 @@
         <v>401</v>
       </c>
       <c r="E270" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L270" t="s">
         <v>32</v>
@@ -7328,7 +7392,7 @@
         <v>407</v>
       </c>
       <c r="E271" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L271" t="s">
         <v>197</v>
@@ -7348,7 +7412,7 @@
         <v>408</v>
       </c>
       <c r="E272" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L272" t="s">
         <v>68</v>
@@ -7365,7 +7429,7 @@
         <v>423</v>
       </c>
       <c r="E273" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L273" t="s">
         <v>424</v>
@@ -7385,7 +7449,7 @@
         <v>429</v>
       </c>
       <c r="E274" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L274" t="s">
         <v>32</v>
@@ -7402,7 +7466,7 @@
         <v>433</v>
       </c>
       <c r="E275" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L275" t="s">
         <v>22</v>
@@ -7419,7 +7483,7 @@
         <v>436</v>
       </c>
       <c r="E276" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L276" t="s">
         <v>140</v>
@@ -7436,7 +7500,7 @@
         <v>437</v>
       </c>
       <c r="E277" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L277" t="s">
         <v>82</v>
@@ -7453,7 +7517,7 @@
         <v>439</v>
       </c>
       <c r="E278" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L278" t="s">
         <v>142</v>
@@ -7470,7 +7534,10 @@
         <v>440</v>
       </c>
       <c r="E279" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="G279" t="s">
+        <v>564</v>
       </c>
       <c r="L279" t="s">
         <v>82</v>
@@ -7490,7 +7557,7 @@
         <v>441</v>
       </c>
       <c r="E280" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L280" t="s">
         <v>442</v>
@@ -7507,7 +7574,7 @@
         <v>448</v>
       </c>
       <c r="E281" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L281" t="s">
         <v>11</v>
@@ -7527,7 +7594,7 @@
         <v>451</v>
       </c>
       <c r="E282" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L282" t="s">
         <v>32</v>
@@ -7547,7 +7614,7 @@
         <v>454</v>
       </c>
       <c r="E283" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L283" t="s">
         <v>22</v>
@@ -7564,7 +7631,7 @@
         <v>456</v>
       </c>
       <c r="E284" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L284" t="s">
         <v>160</v>
@@ -7581,7 +7648,7 @@
         <v>458</v>
       </c>
       <c r="E285" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L285" t="s">
         <v>459</v>
@@ -7598,7 +7665,7 @@
         <v>461</v>
       </c>
       <c r="E286" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L286" t="s">
         <v>462</v>
@@ -7615,7 +7682,7 @@
         <v>464</v>
       </c>
       <c r="E287" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L287" t="s">
         <v>465</v>
@@ -7632,7 +7699,7 @@
         <v>560</v>
       </c>
       <c r="E288" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L288" t="s">
         <v>140</v>
@@ -7649,7 +7716,7 @@
         <v>472</v>
       </c>
       <c r="E289" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L289" t="s">
         <v>178</v>
@@ -7666,7 +7733,7 @@
         <v>473</v>
       </c>
       <c r="E290" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L290" t="s">
         <v>82</v>
@@ -7683,7 +7750,7 @@
         <v>474</v>
       </c>
       <c r="E291" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L291" t="s">
         <v>114</v>
@@ -7700,7 +7767,7 @@
         <v>478</v>
       </c>
       <c r="E292" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L292" t="s">
         <v>124</v>
@@ -7717,7 +7784,7 @@
         <v>483</v>
       </c>
       <c r="E293" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L293" t="s">
         <v>48</v>
@@ -7734,7 +7801,7 @@
         <v>484</v>
       </c>
       <c r="E294" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L294" t="s">
         <v>216</v>
@@ -7751,7 +7818,10 @@
         <v>485</v>
       </c>
       <c r="E295" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="G295" t="s">
+        <v>564</v>
       </c>
       <c r="L295" t="s">
         <v>486</v>
@@ -7768,7 +7838,7 @@
         <v>490</v>
       </c>
       <c r="E296" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L296" t="s">
         <v>491</v>
@@ -7788,7 +7858,10 @@
         <v>492</v>
       </c>
       <c r="E297" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="G297" t="s">
+        <v>564</v>
       </c>
       <c r="L297" t="s">
         <v>491</v>
@@ -7805,7 +7878,7 @@
         <v>493</v>
       </c>
       <c r="E298" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L298" t="s">
         <v>248</v>
@@ -7825,7 +7898,7 @@
         <v>494</v>
       </c>
       <c r="E299" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L299" t="s">
         <v>279</v>
@@ -7842,7 +7915,7 @@
         <v>495</v>
       </c>
       <c r="E300" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L300" t="s">
         <v>248</v>
@@ -7862,7 +7935,7 @@
         <v>496</v>
       </c>
       <c r="E301" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L301" t="s">
         <v>279</v>
@@ -7879,7 +7952,7 @@
         <v>497</v>
       </c>
       <c r="E302" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L302" t="s">
         <v>491</v>
@@ -7896,7 +7969,7 @@
         <v>498</v>
       </c>
       <c r="E303" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L303" t="s">
         <v>499</v>
@@ -7913,7 +7986,7 @@
         <v>501</v>
       </c>
       <c r="E304" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L304" t="s">
         <v>48</v>
@@ -7930,7 +8003,7 @@
         <v>502</v>
       </c>
       <c r="E305" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L305" t="s">
         <v>197</v>
@@ -7947,7 +8020,7 @@
         <v>510</v>
       </c>
       <c r="E306" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L306" t="s">
         <v>114</v>
@@ -7964,7 +8037,7 @@
         <v>516</v>
       </c>
       <c r="E307" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L307" t="s">
         <v>82</v>
@@ -7981,7 +8054,7 @@
         <v>4</v>
       </c>
       <c r="E308" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L308" t="s">
         <v>5</v>
@@ -7998,7 +8071,7 @@
         <v>18</v>
       </c>
       <c r="E309" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L309" t="s">
         <v>19</v>
@@ -8018,7 +8091,7 @@
         <v>20</v>
       </c>
       <c r="E310" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L310" t="s">
         <v>11</v>
@@ -8035,7 +8108,7 @@
         <v>67</v>
       </c>
       <c r="E311" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L311" t="s">
         <v>68</v>
@@ -8052,7 +8125,7 @@
         <v>75</v>
       </c>
       <c r="E312" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L312" t="s">
         <v>11</v>
@@ -8072,7 +8145,7 @@
         <v>92</v>
       </c>
       <c r="E313" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L313" t="s">
         <v>82</v>
@@ -8089,7 +8162,7 @@
         <v>117</v>
       </c>
       <c r="E314" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L314" t="s">
         <v>118</v>
@@ -8106,7 +8179,7 @@
         <v>130</v>
       </c>
       <c r="E315" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L315" t="s">
         <v>131</v>
@@ -8123,7 +8196,7 @@
         <v>139</v>
       </c>
       <c r="E316" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L316" t="s">
         <v>140</v>
@@ -8140,7 +8213,7 @@
         <v>141</v>
       </c>
       <c r="E317" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L317" t="s">
         <v>142</v>
@@ -8157,7 +8230,7 @@
         <v>144</v>
       </c>
       <c r="E318" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L318" t="s">
         <v>142</v>
@@ -8174,7 +8247,7 @@
         <v>147</v>
       </c>
       <c r="E319" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L319" t="s">
         <v>142</v>
@@ -8191,7 +8264,7 @@
         <v>148</v>
       </c>
       <c r="E320" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L320" t="s">
         <v>142</v>
@@ -8208,7 +8281,7 @@
         <v>149</v>
       </c>
       <c r="E321" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L321" t="s">
         <v>142</v>
@@ -8225,7 +8298,7 @@
         <v>150</v>
       </c>
       <c r="E322" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L322" t="s">
         <v>142</v>
@@ -8245,7 +8318,7 @@
         <v>153</v>
       </c>
       <c r="E323" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L323" t="s">
         <v>142</v>
@@ -8265,7 +8338,7 @@
         <v>154</v>
       </c>
       <c r="E324" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L324" t="s">
         <v>142</v>
@@ -8282,7 +8355,7 @@
         <v>155</v>
       </c>
       <c r="E325" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L325" t="s">
         <v>156</v>
@@ -8299,7 +8372,7 @@
         <v>163</v>
       </c>
       <c r="E326" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L326" t="s">
         <v>82</v>
@@ -8316,7 +8389,7 @@
         <v>164</v>
       </c>
       <c r="E327" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L327" t="s">
         <v>140</v>
@@ -8333,7 +8406,7 @@
         <v>172</v>
       </c>
       <c r="E328" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L328" t="s">
         <v>142</v>
@@ -8350,7 +8423,7 @@
         <v>198</v>
       </c>
       <c r="E329" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L329" t="s">
         <v>142</v>
@@ -8367,7 +8440,7 @@
         <v>199</v>
       </c>
       <c r="E330" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L330" t="s">
         <v>142</v>
@@ -8384,7 +8457,7 @@
         <v>210</v>
       </c>
       <c r="E331" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L331" t="s">
         <v>142</v>
@@ -8401,7 +8474,7 @@
         <v>211</v>
       </c>
       <c r="E332" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L332" t="s">
         <v>11</v>
@@ -8418,7 +8491,7 @@
         <v>247</v>
       </c>
       <c r="E333" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L333" t="s">
         <v>248</v>
@@ -8435,7 +8508,7 @@
         <v>265</v>
       </c>
       <c r="E334" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L334" t="s">
         <v>140</v>
@@ -8452,7 +8525,7 @@
         <v>267</v>
       </c>
       <c r="E335" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L335" t="s">
         <v>142</v>
@@ -8469,7 +8542,7 @@
         <v>272</v>
       </c>
       <c r="E336" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L336" t="s">
         <v>273</v>
@@ -8486,7 +8559,7 @@
         <v>274</v>
       </c>
       <c r="E337" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L337" t="s">
         <v>275</v>
@@ -8503,7 +8576,7 @@
         <v>276</v>
       </c>
       <c r="E338" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L338" t="s">
         <v>142</v>
@@ -8520,7 +8593,7 @@
         <v>289</v>
       </c>
       <c r="E339" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L339" t="s">
         <v>156</v>
@@ -8537,7 +8610,7 @@
         <v>302</v>
       </c>
       <c r="E340" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L340" t="s">
         <v>142</v>
@@ -8557,7 +8630,7 @@
         <v>319</v>
       </c>
       <c r="E341" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L341" t="s">
         <v>137</v>
@@ -8574,7 +8647,7 @@
         <v>324</v>
       </c>
       <c r="E342" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L342" t="s">
         <v>142</v>
@@ -8591,7 +8664,7 @@
         <v>327</v>
       </c>
       <c r="E343" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L343" t="s">
         <v>328</v>
@@ -8608,7 +8681,7 @@
         <v>329</v>
       </c>
       <c r="E344" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L344" t="s">
         <v>142</v>
@@ -8625,7 +8698,7 @@
         <v>330</v>
       </c>
       <c r="E345" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L345" t="s">
         <v>140</v>
@@ -8642,7 +8715,7 @@
         <v>334</v>
       </c>
       <c r="E346" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L346" t="s">
         <v>142</v>
@@ -8662,7 +8735,7 @@
         <v>335</v>
       </c>
       <c r="E347" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L347" t="s">
         <v>336</v>
@@ -8682,7 +8755,7 @@
         <v>340</v>
       </c>
       <c r="E348" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L348" t="s">
         <v>114</v>
@@ -8699,7 +8772,7 @@
         <v>347</v>
       </c>
       <c r="E349" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L349" t="s">
         <v>142</v>
@@ -8716,7 +8789,7 @@
         <v>362</v>
       </c>
       <c r="E350" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L350" t="s">
         <v>363</v>
@@ -8733,7 +8806,7 @@
         <v>367</v>
       </c>
       <c r="E351" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L351" t="s">
         <v>368</v>
@@ -8750,7 +8823,7 @@
         <v>393</v>
       </c>
       <c r="E352" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L352" t="s">
         <v>140</v>
@@ -8767,7 +8840,7 @@
         <v>395</v>
       </c>
       <c r="E353" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L353" t="s">
         <v>142</v>
@@ -8784,7 +8857,7 @@
         <v>396</v>
       </c>
       <c r="E354" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L354" t="s">
         <v>142</v>
@@ -8804,7 +8877,7 @@
         <v>397</v>
       </c>
       <c r="E355" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L355" t="s">
         <v>137</v>
@@ -8821,7 +8894,7 @@
         <v>399</v>
       </c>
       <c r="E356" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L356" t="s">
         <v>156</v>
@@ -8841,7 +8914,7 @@
         <v>406</v>
       </c>
       <c r="E357" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L357" t="s">
         <v>142</v>
@@ -8858,7 +8931,7 @@
         <v>409</v>
       </c>
       <c r="E358" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L358" t="s">
         <v>142</v>
@@ -8875,7 +8948,7 @@
         <v>411</v>
       </c>
       <c r="E359" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L359" t="s">
         <v>140</v>
@@ -8895,7 +8968,7 @@
         <v>412</v>
       </c>
       <c r="E360" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L360" t="s">
         <v>131</v>
@@ -8915,7 +8988,7 @@
         <v>418</v>
       </c>
       <c r="E361" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L361" t="s">
         <v>140</v>
@@ -8932,7 +9005,7 @@
         <v>438</v>
       </c>
       <c r="E362" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L362" t="s">
         <v>142</v>
@@ -8949,7 +9022,7 @@
         <v>443</v>
       </c>
       <c r="E363" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L363" t="s">
         <v>142</v>
@@ -8966,7 +9039,7 @@
         <v>444</v>
       </c>
       <c r="E364" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L364" t="s">
         <v>142</v>
@@ -8983,7 +9056,7 @@
         <v>445</v>
       </c>
       <c r="E365" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L365" t="s">
         <v>50</v>
@@ -9000,7 +9073,10 @@
         <v>446</v>
       </c>
       <c r="E366" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="G366" t="s">
+        <v>564</v>
       </c>
       <c r="L366" t="s">
         <v>197</v>
@@ -9017,7 +9093,7 @@
         <v>447</v>
       </c>
       <c r="E367" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L367" t="s">
         <v>140</v>
@@ -9034,13 +9110,13 @@
         <v>460</v>
       </c>
       <c r="E368" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L368" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>3</v>
       </c>
@@ -9051,13 +9127,13 @@
         <v>468</v>
       </c>
       <c r="E369" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L369" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>3</v>
       </c>
@@ -9068,13 +9144,13 @@
         <v>469</v>
       </c>
       <c r="E370" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L370" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>3</v>
       </c>
@@ -9085,13 +9161,13 @@
         <v>481</v>
       </c>
       <c r="E371" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L371" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>3</v>
       </c>
@@ -9102,13 +9178,13 @@
         <v>487</v>
       </c>
       <c r="E372" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L372" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>3</v>
       </c>
@@ -9122,13 +9198,13 @@
         <v>500</v>
       </c>
       <c r="E373" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L373" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>126</v>
       </c>
@@ -9139,13 +9215,13 @@
         <v>127</v>
       </c>
       <c r="E374" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L374" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>126</v>
       </c>
@@ -9156,13 +9232,13 @@
         <v>205</v>
       </c>
       <c r="E375" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L375" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>126</v>
       </c>
@@ -9173,13 +9249,13 @@
         <v>239</v>
       </c>
       <c r="E376" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L376" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>126</v>
       </c>
@@ -9190,13 +9266,13 @@
         <v>283</v>
       </c>
       <c r="E377" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L377" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>126</v>
       </c>
@@ -9207,10 +9283,178 @@
         <v>466</v>
       </c>
       <c r="E378" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L378" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="379" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B379" t="s">
+        <v>525</v>
+      </c>
+      <c r="D379" t="s">
+        <v>578</v>
+      </c>
+      <c r="G379" t="s">
+        <v>564</v>
+      </c>
+      <c r="M379" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="380" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B380" t="s">
+        <v>525</v>
+      </c>
+      <c r="D380" t="s">
+        <v>579</v>
+      </c>
+      <c r="G380" t="s">
+        <v>564</v>
+      </c>
+      <c r="M380" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="381" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B381" t="s">
+        <v>525</v>
+      </c>
+      <c r="D381" t="s">
+        <v>580</v>
+      </c>
+      <c r="G381" t="s">
+        <v>564</v>
+      </c>
+      <c r="M381" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="382" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B382" t="s">
+        <v>525</v>
+      </c>
+      <c r="D382" t="s">
+        <v>581</v>
+      </c>
+      <c r="G382" t="s">
+        <v>564</v>
+      </c>
+      <c r="M382" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B383" t="s">
+        <v>555</v>
+      </c>
+      <c r="D383" t="s">
+        <v>582</v>
+      </c>
+      <c r="G383" t="s">
+        <v>564</v>
+      </c>
+      <c r="M383" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="384" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B384" t="s">
+        <v>555</v>
+      </c>
+      <c r="D384" t="s">
+        <v>583</v>
+      </c>
+      <c r="G384" t="s">
+        <v>564</v>
+      </c>
+      <c r="M384" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="385" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B385" t="s">
+        <v>554</v>
+      </c>
+      <c r="D385" t="s">
+        <v>576</v>
+      </c>
+      <c r="G385" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="386" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B386" t="s">
+        <v>555</v>
+      </c>
+      <c r="D386" t="s">
+        <v>584</v>
+      </c>
+      <c r="G386" t="s">
+        <v>564</v>
+      </c>
+      <c r="M386" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="387" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B387" t="s">
+        <v>555</v>
+      </c>
+      <c r="D387" t="s">
+        <v>585</v>
+      </c>
+      <c r="G387" t="s">
+        <v>564</v>
+      </c>
+      <c r="M387" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="388" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B388" t="s">
+        <v>545</v>
+      </c>
+      <c r="D388" t="s">
+        <v>586</v>
+      </c>
+      <c r="G388" t="s">
+        <v>564</v>
+      </c>
+      <c r="M388" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="389" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B389" t="s">
+        <v>545</v>
+      </c>
+      <c r="C389" t="s">
+        <v>555</v>
+      </c>
+      <c r="D389" t="s">
+        <v>587</v>
+      </c>
+      <c r="G389" t="s">
+        <v>564</v>
+      </c>
+      <c r="M389" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="390" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B390" t="s">
+        <v>519</v>
+      </c>
+      <c r="D390" t="s">
+        <v>588</v>
+      </c>
+      <c r="G390" t="s">
+        <v>564</v>
+      </c>
+      <c r="M390" t="s">
+        <v>577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean-code rules completely in list
</commit_message>
<xml_diff>
--- a/files/sq_rules.xlsx
+++ b/files/sq_rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2015" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="619">
   <si>
     <t>blocker</t>
   </si>
@@ -1781,6 +1781,96 @@
   </si>
   <si>
     <t>Auf der richtigen Abstraktionsebene Codieren</t>
+  </si>
+  <si>
+    <t>Basisklassen sollten nicht von abgeleiteten Klassen abhängen</t>
+  </si>
+  <si>
+    <t>Möglichst kleine Interfaces</t>
+  </si>
+  <si>
+    <t>Kein ungenutzter Code</t>
+  </si>
+  <si>
+    <t>Geringe vertikale Gültigkeit von Variablen und Methoden</t>
+  </si>
+  <si>
+    <t>konsistente Benamung</t>
+  </si>
+  <si>
+    <t>Keine überflüssige Kopplung</t>
+  </si>
+  <si>
+    <t>Möglichst kein "Funktionsneid"</t>
+  </si>
+  <si>
+    <t>sprechende Namen für alles - keine Ungarische Notation usw.</t>
+  </si>
+  <si>
+    <t>Zuständigkeiten sinnvoll zuordnen und durch entsprechende Namen kennzeichnen</t>
+  </si>
+  <si>
+    <t>Nur Methoden die nie polymorphes Verhalten haben können als Static definieren</t>
+  </si>
+  <si>
+    <t>Zwischenergebnisse in Aussagekräftig benannten Variablen ablegen</t>
+  </si>
+  <si>
+    <t>Funktionsweise des implementierten Algorithmus verstehen</t>
+  </si>
+  <si>
+    <t>Logische Abhängigkeiten in Physischen Abhängigkeiten festschreiben</t>
+  </si>
+  <si>
+    <t>Switch-Anweisungen vermeiden - stattdessen polymorphismus</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Präzise implementieren</t>
+  </si>
+  <si>
+    <t>Struktur wichtiger als Konvention</t>
+  </si>
+  <si>
+    <t>Nicht triviale Bedingungen in Methoden einkapseln zur besseren Lesbarkeit der Anweisungen</t>
+  </si>
+  <si>
+    <t>Negative Bedingungen vermeiden</t>
+  </si>
+  <si>
+    <t>Eine Aufgabe pro Methode</t>
+  </si>
+  <si>
+    <t>Keine verborgene zeitliche Abhängigkeit (Reihenfolge von Methodenaufrufen)</t>
+  </si>
+  <si>
+    <t>Keine willkürliche Strukturierung</t>
+  </si>
+  <si>
+    <t>Grenzbedingungen (z.B. +/- 1) in extra Variable einkapseln</t>
+  </si>
+  <si>
+    <t>Nur EINE Stufe pro Methode (eine Abstraktionsebene)</t>
+  </si>
+  <si>
+    <t>Konfigurierbare Konstanten / Variablen auf hoher Abstraktionsebene ansiedeln</t>
+  </si>
+  <si>
+    <t>Transitivie Methodenaufrufe vermeiden - "a.getB().getC()"</t>
+  </si>
+  <si>
+    <t>Wildcard imports nutzen wenn mehr als zwei Klassen aus Package</t>
+  </si>
+  <si>
+    <t>Gegenteil von SQ-Regel</t>
+  </si>
+  <si>
+    <t>Keine Konstanten vererben</t>
+  </si>
+  <si>
+    <t>Enums gegenüber Konstanten bevorzugen</t>
   </si>
 </sst>
 </file>
@@ -2610,10 +2700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M390"/>
+  <dimension ref="A1:M417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D358" workbookViewId="0">
-      <selection activeCell="D358" sqref="D358"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D389" sqref="D389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2628,8 +2718,8 @@
     <col min="9" max="9" width="8.5546875" customWidth="1"/>
     <col min="10" max="10" width="9.44140625" customWidth="1"/>
     <col min="11" max="11" width="7.21875" customWidth="1"/>
-    <col min="12" max="12" width="51" customWidth="1"/>
-    <col min="13" max="13" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="58.109375" customWidth="1"/>
+    <col min="13" max="13" width="44.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -5624,6 +5714,9 @@
       <c r="E172" t="s">
         <v>564</v>
       </c>
+      <c r="G172" t="s">
+        <v>564</v>
+      </c>
       <c r="L172" t="s">
         <v>11</v>
       </c>
@@ -5854,6 +5947,9 @@
       <c r="E185" t="s">
         <v>564</v>
       </c>
+      <c r="G185" t="s">
+        <v>564</v>
+      </c>
       <c r="L185" t="s">
         <v>114</v>
       </c>
@@ -5983,7 +6079,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>9</v>
       </c>
@@ -6000,7 +6096,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>9</v>
       </c>
@@ -6017,7 +6113,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>9</v>
       </c>
@@ -6034,7 +6130,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>9</v>
       </c>
@@ -6054,7 +6150,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>9</v>
       </c>
@@ -6071,7 +6167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>9</v>
       </c>
@@ -6088,7 +6184,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>9</v>
       </c>
@@ -6101,11 +6197,17 @@
       <c r="E199" t="s">
         <v>564</v>
       </c>
+      <c r="G199" t="s">
+        <v>564</v>
+      </c>
       <c r="L199" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M199" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -6125,7 +6227,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -6142,7 +6244,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>9</v>
       </c>
@@ -6162,7 +6264,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>9</v>
       </c>
@@ -6179,7 +6281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>9</v>
       </c>
@@ -6196,7 +6298,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>9</v>
       </c>
@@ -6216,7 +6318,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>9</v>
       </c>
@@ -6236,7 +6338,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>9</v>
       </c>
@@ -6253,7 +6355,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>9</v>
       </c>
@@ -6473,6 +6575,9 @@
       <c r="E220" t="s">
         <v>564</v>
       </c>
+      <c r="G220" t="s">
+        <v>564</v>
+      </c>
       <c r="L220" t="s">
         <v>8</v>
       </c>
@@ -6808,6 +6913,9 @@
       <c r="E239" t="s">
         <v>564</v>
       </c>
+      <c r="G239" t="s">
+        <v>564</v>
+      </c>
       <c r="L239" t="s">
         <v>11</v>
       </c>
@@ -7502,6 +7610,9 @@
       <c r="E277" t="s">
         <v>564</v>
       </c>
+      <c r="G277" t="s">
+        <v>564</v>
+      </c>
       <c r="L277" t="s">
         <v>82</v>
       </c>
@@ -7684,6 +7795,9 @@
       <c r="E287" t="s">
         <v>564</v>
       </c>
+      <c r="G287" t="s">
+        <v>564</v>
+      </c>
       <c r="L287" t="s">
         <v>465</v>
       </c>
@@ -7840,6 +7954,9 @@
       <c r="E296" t="s">
         <v>564</v>
       </c>
+      <c r="G296" t="s">
+        <v>564</v>
+      </c>
       <c r="L296" t="s">
         <v>491</v>
       </c>
@@ -7880,6 +7997,9 @@
       <c r="E298" t="s">
         <v>564</v>
       </c>
+      <c r="G298" t="s">
+        <v>564</v>
+      </c>
       <c r="L298" t="s">
         <v>248</v>
       </c>
@@ -7900,6 +8020,9 @@
       <c r="E299" t="s">
         <v>564</v>
       </c>
+      <c r="G299" t="s">
+        <v>564</v>
+      </c>
       <c r="L299" t="s">
         <v>279</v>
       </c>
@@ -7917,6 +8040,9 @@
       <c r="E300" t="s">
         <v>564</v>
       </c>
+      <c r="G300" t="s">
+        <v>564</v>
+      </c>
       <c r="L300" t="s">
         <v>248</v>
       </c>
@@ -7937,6 +8063,9 @@
       <c r="E301" t="s">
         <v>564</v>
       </c>
+      <c r="G301" t="s">
+        <v>564</v>
+      </c>
       <c r="L301" t="s">
         <v>279</v>
       </c>
@@ -7952,6 +8081,9 @@
         <v>497</v>
       </c>
       <c r="E302" t="s">
+        <v>564</v>
+      </c>
+      <c r="G302" t="s">
         <v>564</v>
       </c>
       <c r="L302" t="s">
@@ -8215,6 +8347,9 @@
       <c r="E317" t="s">
         <v>564</v>
       </c>
+      <c r="G317" t="s">
+        <v>564</v>
+      </c>
       <c r="L317" t="s">
         <v>142</v>
       </c>
@@ -8232,6 +8367,9 @@
       <c r="E318" t="s">
         <v>564</v>
       </c>
+      <c r="G318" t="s">
+        <v>564</v>
+      </c>
       <c r="L318" t="s">
         <v>142</v>
       </c>
@@ -8266,6 +8404,9 @@
       <c r="E320" t="s">
         <v>564</v>
       </c>
+      <c r="G320" t="s">
+        <v>564</v>
+      </c>
       <c r="L320" t="s">
         <v>142</v>
       </c>
@@ -8283,6 +8424,9 @@
       <c r="E321" t="s">
         <v>564</v>
       </c>
+      <c r="G321" t="s">
+        <v>564</v>
+      </c>
       <c r="L321" t="s">
         <v>142</v>
       </c>
@@ -8357,6 +8501,9 @@
       <c r="E325" t="s">
         <v>564</v>
       </c>
+      <c r="G325" t="s">
+        <v>564</v>
+      </c>
       <c r="L325" t="s">
         <v>156</v>
       </c>
@@ -8408,6 +8555,9 @@
       <c r="E328" t="s">
         <v>564</v>
       </c>
+      <c r="G328" t="s">
+        <v>564</v>
+      </c>
       <c r="L328" t="s">
         <v>142</v>
       </c>
@@ -8425,6 +8575,9 @@
       <c r="E329" t="s">
         <v>564</v>
       </c>
+      <c r="G329" t="s">
+        <v>564</v>
+      </c>
       <c r="L329" t="s">
         <v>142</v>
       </c>
@@ -8442,6 +8595,9 @@
       <c r="E330" t="s">
         <v>564</v>
       </c>
+      <c r="G330" t="s">
+        <v>564</v>
+      </c>
       <c r="L330" t="s">
         <v>142</v>
       </c>
@@ -8459,6 +8615,9 @@
       <c r="E331" t="s">
         <v>564</v>
       </c>
+      <c r="G331" t="s">
+        <v>564</v>
+      </c>
       <c r="L331" t="s">
         <v>142</v>
       </c>
@@ -8493,6 +8652,9 @@
       <c r="E333" t="s">
         <v>564</v>
       </c>
+      <c r="G333" t="s">
+        <v>564</v>
+      </c>
       <c r="L333" t="s">
         <v>248</v>
       </c>
@@ -8527,6 +8689,9 @@
       <c r="E335" t="s">
         <v>564</v>
       </c>
+      <c r="G335" t="s">
+        <v>564</v>
+      </c>
       <c r="L335" t="s">
         <v>142</v>
       </c>
@@ -8595,6 +8760,9 @@
       <c r="E339" t="s">
         <v>564</v>
       </c>
+      <c r="G339" t="s">
+        <v>564</v>
+      </c>
       <c r="L339" t="s">
         <v>156</v>
       </c>
@@ -8612,6 +8780,9 @@
       <c r="E340" t="s">
         <v>564</v>
       </c>
+      <c r="G340" t="s">
+        <v>564</v>
+      </c>
       <c r="L340" t="s">
         <v>142</v>
       </c>
@@ -8683,6 +8854,9 @@
       <c r="E344" t="s">
         <v>564</v>
       </c>
+      <c r="G344" t="s">
+        <v>564</v>
+      </c>
       <c r="L344" t="s">
         <v>142</v>
       </c>
@@ -8717,6 +8891,9 @@
       <c r="E346" t="s">
         <v>564</v>
       </c>
+      <c r="G346" t="s">
+        <v>564</v>
+      </c>
       <c r="L346" t="s">
         <v>142</v>
       </c>
@@ -8757,6 +8934,9 @@
       <c r="E348" t="s">
         <v>564</v>
       </c>
+      <c r="G348" t="s">
+        <v>564</v>
+      </c>
       <c r="L348" t="s">
         <v>114</v>
       </c>
@@ -8774,6 +8954,9 @@
       <c r="E349" t="s">
         <v>564</v>
       </c>
+      <c r="G349" t="s">
+        <v>564</v>
+      </c>
       <c r="L349" t="s">
         <v>142</v>
       </c>
@@ -8842,6 +9025,9 @@
       <c r="E353" t="s">
         <v>564</v>
       </c>
+      <c r="G353" t="s">
+        <v>564</v>
+      </c>
       <c r="L353" t="s">
         <v>142</v>
       </c>
@@ -9007,6 +9193,9 @@
       <c r="E362" t="s">
         <v>564</v>
       </c>
+      <c r="G362" t="s">
+        <v>564</v>
+      </c>
       <c r="L362" t="s">
         <v>142</v>
       </c>
@@ -9041,6 +9230,9 @@
       <c r="E364" t="s">
         <v>564</v>
       </c>
+      <c r="G364" t="s">
+        <v>564</v>
+      </c>
       <c r="L364" t="s">
         <v>142</v>
       </c>
@@ -9180,6 +9372,9 @@
       <c r="E372" t="s">
         <v>564</v>
       </c>
+      <c r="G372" t="s">
+        <v>564</v>
+      </c>
       <c r="L372" t="s">
         <v>142</v>
       </c>
@@ -9200,6 +9395,9 @@
       <c r="E373" t="s">
         <v>564</v>
       </c>
+      <c r="G373" t="s">
+        <v>564</v>
+      </c>
       <c r="L373" t="s">
         <v>279</v>
       </c>
@@ -9454,6 +9652,369 @@
         <v>564</v>
       </c>
       <c r="M390" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="391" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B391" t="s">
+        <v>519</v>
+      </c>
+      <c r="D391" t="s">
+        <v>589</v>
+      </c>
+      <c r="G391" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="392" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B392" t="s">
+        <v>531</v>
+      </c>
+      <c r="D392" t="s">
+        <v>590</v>
+      </c>
+      <c r="G392" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="393" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B393" t="s">
+        <v>558</v>
+      </c>
+      <c r="D393" t="s">
+        <v>591</v>
+      </c>
+      <c r="G393" t="s">
+        <v>564</v>
+      </c>
+      <c r="M393" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="394" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B394" t="s">
+        <v>555</v>
+      </c>
+      <c r="D394" t="s">
+        <v>592</v>
+      </c>
+      <c r="G394" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="395" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B395" t="s">
+        <v>537</v>
+      </c>
+      <c r="D395" t="s">
+        <v>593</v>
+      </c>
+      <c r="G395" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="396" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B396" t="s">
+        <v>547</v>
+      </c>
+      <c r="D396" t="s">
+        <v>594</v>
+      </c>
+      <c r="G396" t="s">
+        <v>564</v>
+      </c>
+      <c r="M396" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="397" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B397" t="s">
+        <v>547</v>
+      </c>
+      <c r="D397" t="s">
+        <v>595</v>
+      </c>
+      <c r="G397" t="s">
+        <v>564</v>
+      </c>
+      <c r="M397" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="398" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B398" t="s">
+        <v>537</v>
+      </c>
+      <c r="D398" t="s">
+        <v>596</v>
+      </c>
+      <c r="G398" t="s">
+        <v>564</v>
+      </c>
+      <c r="M398" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="399" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B399" t="s">
+        <v>537</v>
+      </c>
+      <c r="C399" t="s">
+        <v>555</v>
+      </c>
+      <c r="D399" t="s">
+        <v>597</v>
+      </c>
+      <c r="G399" t="s">
+        <v>564</v>
+      </c>
+      <c r="M399" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="400" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B400" t="s">
+        <v>535</v>
+      </c>
+      <c r="C400" t="s">
+        <v>554</v>
+      </c>
+      <c r="D400" t="s">
+        <v>598</v>
+      </c>
+      <c r="G400" t="s">
+        <v>564</v>
+      </c>
+      <c r="M400" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="401" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B401" t="s">
+        <v>537</v>
+      </c>
+      <c r="C401" t="s">
+        <v>530</v>
+      </c>
+      <c r="D401" t="s">
+        <v>599</v>
+      </c>
+      <c r="G401" t="s">
+        <v>564</v>
+      </c>
+      <c r="M401" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="402" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B402" t="s">
+        <v>603</v>
+      </c>
+      <c r="D402" t="s">
+        <v>600</v>
+      </c>
+      <c r="G402" t="s">
+        <v>564</v>
+      </c>
+      <c r="M402" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="403" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B403" t="s">
+        <v>547</v>
+      </c>
+      <c r="D403" t="s">
+        <v>601</v>
+      </c>
+      <c r="G403" t="s">
+        <v>564</v>
+      </c>
+      <c r="M403" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="404" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B404" t="s">
+        <v>529</v>
+      </c>
+      <c r="D404" t="s">
+        <v>602</v>
+      </c>
+      <c r="G404" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="405" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B405" t="s">
+        <v>603</v>
+      </c>
+      <c r="D405" t="s">
+        <v>604</v>
+      </c>
+      <c r="G405" t="s">
+        <v>564</v>
+      </c>
+      <c r="M405" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="406" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B406" t="s">
+        <v>555</v>
+      </c>
+      <c r="D406" t="s">
+        <v>605</v>
+      </c>
+      <c r="G406" t="s">
+        <v>564</v>
+      </c>
+      <c r="M406" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="407" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B407" t="s">
+        <v>529</v>
+      </c>
+      <c r="D407" t="s">
+        <v>606</v>
+      </c>
+      <c r="G407" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="408" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B408" t="s">
+        <v>529</v>
+      </c>
+      <c r="D408" t="s">
+        <v>607</v>
+      </c>
+      <c r="G408" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="409" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B409" t="s">
+        <v>554</v>
+      </c>
+      <c r="D409" t="s">
+        <v>608</v>
+      </c>
+      <c r="G409" t="s">
+        <v>564</v>
+      </c>
+      <c r="M409" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="410" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B410" t="s">
+        <v>547</v>
+      </c>
+      <c r="D410" t="s">
+        <v>609</v>
+      </c>
+      <c r="G410" t="s">
+        <v>564</v>
+      </c>
+      <c r="M410" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="411" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B411" t="s">
+        <v>555</v>
+      </c>
+      <c r="D411" t="s">
+        <v>610</v>
+      </c>
+      <c r="G411" t="s">
+        <v>564</v>
+      </c>
+      <c r="M411" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="412" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B412" t="s">
+        <v>530</v>
+      </c>
+      <c r="D412" t="s">
+        <v>611</v>
+      </c>
+      <c r="G412" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="413" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B413" t="s">
+        <v>555</v>
+      </c>
+      <c r="C413" t="s">
+        <v>530</v>
+      </c>
+      <c r="D413" t="s">
+        <v>613</v>
+      </c>
+      <c r="G413" t="s">
+        <v>564</v>
+      </c>
+      <c r="M413" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="414" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B414" t="s">
+        <v>555</v>
+      </c>
+      <c r="C414" t="s">
+        <v>554</v>
+      </c>
+      <c r="D414" t="s">
+        <v>614</v>
+      </c>
+      <c r="G414" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="415" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B415" t="s">
+        <v>559</v>
+      </c>
+      <c r="D415" t="s">
+        <v>615</v>
+      </c>
+      <c r="G415" t="s">
+        <v>564</v>
+      </c>
+      <c r="M415" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="416" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B416" t="s">
+        <v>519</v>
+      </c>
+      <c r="D416" t="s">
+        <v>617</v>
+      </c>
+      <c r="G416" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="417" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B417" t="s">
+        <v>546</v>
+      </c>
+      <c r="D417" t="s">
+        <v>618</v>
+      </c>
+      <c r="G417" t="s">
+        <v>564</v>
+      </c>
+      <c r="M417" t="s">
         <v>577</v>
       </c>
     </row>

</xml_diff>

<commit_message>
half of the Java-Style-Book rules in excel
</commit_message>
<xml_diff>
--- a/files/sq_rules.xlsx
+++ b/files/sq_rules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="635">
   <si>
     <t>blocker</t>
   </si>
@@ -1804,9 +1804,6 @@
     <t>Möglichst kein "Funktionsneid"</t>
   </si>
   <si>
-    <t>sprechende Namen für alles - keine Ungarische Notation usw.</t>
-  </si>
-  <si>
     <t>Zuständigkeiten sinnvoll zuordnen und durch entsprechende Namen kennzeichnen</t>
   </si>
   <si>
@@ -1871,6 +1868,57 @@
   </si>
   <si>
     <t>Enums gegenüber Konstanten bevorzugen</t>
+  </si>
+  <si>
+    <t>Use original style when adding something</t>
+  </si>
+  <si>
+    <t>Java-Style-Comment</t>
+  </si>
+  <si>
+    <t>Rules for all Code (Test, prototype, …)</t>
+  </si>
+  <si>
+    <t>(X)</t>
+  </si>
+  <si>
+    <t>Document intended Rule violations</t>
+  </si>
+  <si>
+    <t>Lieber keine dafür sprechende namen</t>
+  </si>
+  <si>
+    <t>Whitespaces around braces, operators, parentheses</t>
+  </si>
+  <si>
+    <t>Blank lines between logical sections, class members, methods and classes</t>
+  </si>
+  <si>
+    <t>Refactor elements with to long names</t>
+  </si>
+  <si>
+    <t>sprechende Namen für alles - keine Ungarische Notation, Bkürzungen, usw.</t>
+  </si>
+  <si>
+    <t>Abkürzungen in zusammengestzten namen nur mit erstem buchstaben groß: getXml</t>
+  </si>
+  <si>
+    <t>use Field names with "this"</t>
+  </si>
+  <si>
+    <t>Consistent comment style</t>
+  </si>
+  <si>
+    <t>Erlaubt!!!</t>
+  </si>
+  <si>
+    <t>Comment everything, completely</t>
+  </si>
+  <si>
+    <t>Erwünscht!!!</t>
+  </si>
+  <si>
+    <t>Unglaublich viele Kommentare schreiben…. Für alles… ALLES!!!</t>
   </si>
 </sst>
 </file>
@@ -2700,10 +2748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M417"/>
+  <dimension ref="A1:N427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D389" sqref="D389"/>
+    <sheetView tabSelected="1" topLeftCell="B398" workbookViewId="0">
+      <selection activeCell="B428" sqref="B428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2720,9 +2768,10 @@
     <col min="11" max="11" width="7.21875" customWidth="1"/>
     <col min="12" max="12" width="58.109375" customWidth="1"/>
     <col min="13" max="13" width="44.77734375" customWidth="1"/>
+    <col min="14" max="14" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>562</v>
       </c>
@@ -2762,8 +2811,11 @@
       <c r="M1" s="1" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2780,7 +2832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2814,7 +2866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2831,7 +2883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2848,7 +2900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2865,7 +2917,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2882,7 +2934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2899,7 +2951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2916,7 +2968,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +2985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2950,7 +3002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2967,7 +3019,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2980,11 +3032,14 @@
       <c r="E14" t="s">
         <v>564</v>
       </c>
+      <c r="K14" t="s">
+        <v>564</v>
+      </c>
       <c r="L14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -3001,7 +3056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -6204,7 +6259,7 @@
         <v>114</v>
       </c>
       <c r="M199" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.3">
@@ -6652,6 +6707,9 @@
       <c r="E224" t="s">
         <v>564</v>
       </c>
+      <c r="G224" t="s">
+        <v>564</v>
+      </c>
       <c r="L224" t="s">
         <v>114</v>
       </c>
@@ -6757,6 +6815,9 @@
       <c r="E230" t="s">
         <v>564</v>
       </c>
+      <c r="G230" t="s">
+        <v>564</v>
+      </c>
       <c r="L230" t="s">
         <v>114</v>
       </c>
@@ -7067,6 +7128,9 @@
       <c r="E247" t="s">
         <v>564</v>
       </c>
+      <c r="J247" t="s">
+        <v>564</v>
+      </c>
       <c r="L247" t="s">
         <v>48</v>
       </c>
@@ -7158,6 +7222,9 @@
       <c r="E252" t="s">
         <v>564</v>
       </c>
+      <c r="G252" t="s">
+        <v>564</v>
+      </c>
       <c r="L252" t="s">
         <v>114</v>
       </c>
@@ -7526,7 +7593,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>9</v>
       </c>
@@ -7542,8 +7609,11 @@
       <c r="L273" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N273" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>9</v>
       </c>
@@ -7563,7 +7633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>9</v>
       </c>
@@ -7580,7 +7650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>9</v>
       </c>
@@ -7597,7 +7667,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>9</v>
       </c>
@@ -7617,7 +7687,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>9</v>
       </c>
@@ -7630,11 +7700,20 @@
       <c r="E278" t="s">
         <v>564</v>
       </c>
+      <c r="K278" t="s">
+        <v>564</v>
+      </c>
       <c r="L278" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M278" t="s">
+        <v>623</v>
+      </c>
+      <c r="N278" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="279" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>9</v>
       </c>
@@ -7654,7 +7733,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>9</v>
       </c>
@@ -7674,7 +7753,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>9</v>
       </c>
@@ -7691,7 +7770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>9</v>
       </c>
@@ -7711,7 +7790,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>9</v>
       </c>
@@ -7731,7 +7810,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>9</v>
       </c>
@@ -7748,7 +7827,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>9</v>
       </c>
@@ -7765,7 +7844,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>9</v>
       </c>
@@ -7782,7 +7861,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>9</v>
       </c>
@@ -7802,7 +7881,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>9</v>
       </c>
@@ -8370,6 +8449,9 @@
       <c r="G318" t="s">
         <v>564</v>
       </c>
+      <c r="K318" t="s">
+        <v>564</v>
+      </c>
       <c r="L318" t="s">
         <v>142</v>
       </c>
@@ -8558,6 +8640,9 @@
       <c r="G328" t="s">
         <v>564</v>
       </c>
+      <c r="K328" t="s">
+        <v>564</v>
+      </c>
       <c r="L328" t="s">
         <v>142</v>
       </c>
@@ -8618,6 +8703,9 @@
       <c r="G331" t="s">
         <v>564</v>
       </c>
+      <c r="K331" t="s">
+        <v>564</v>
+      </c>
       <c r="L331" t="s">
         <v>142</v>
       </c>
@@ -8692,6 +8780,9 @@
       <c r="G335" t="s">
         <v>564</v>
       </c>
+      <c r="K335" t="s">
+        <v>564</v>
+      </c>
       <c r="L335" t="s">
         <v>142</v>
       </c>
@@ -8783,6 +8874,9 @@
       <c r="G340" t="s">
         <v>564</v>
       </c>
+      <c r="K340" t="s">
+        <v>564</v>
+      </c>
       <c r="L340" t="s">
         <v>142</v>
       </c>
@@ -8820,6 +8914,9 @@
       <c r="E342" t="s">
         <v>564</v>
       </c>
+      <c r="K342" t="s">
+        <v>564</v>
+      </c>
       <c r="L342" t="s">
         <v>142</v>
       </c>
@@ -8857,6 +8954,9 @@
       <c r="G344" t="s">
         <v>564</v>
       </c>
+      <c r="K344" t="s">
+        <v>564</v>
+      </c>
       <c r="L344" t="s">
         <v>142</v>
       </c>
@@ -8957,6 +9057,9 @@
       <c r="G349" t="s">
         <v>564</v>
       </c>
+      <c r="K349" t="s">
+        <v>564</v>
+      </c>
       <c r="L349" t="s">
         <v>142</v>
       </c>
@@ -9028,6 +9131,9 @@
       <c r="G353" t="s">
         <v>564</v>
       </c>
+      <c r="K353" t="s">
+        <v>564</v>
+      </c>
       <c r="L353" t="s">
         <v>142</v>
       </c>
@@ -9045,6 +9151,9 @@
       <c r="E354" t="s">
         <v>564</v>
       </c>
+      <c r="K354" t="s">
+        <v>564</v>
+      </c>
       <c r="L354" t="s">
         <v>142</v>
       </c>
@@ -9119,6 +9228,9 @@
       <c r="E358" t="s">
         <v>564</v>
       </c>
+      <c r="K358" t="s">
+        <v>564</v>
+      </c>
       <c r="L358" t="s">
         <v>142</v>
       </c>
@@ -9196,6 +9308,9 @@
       <c r="G362" t="s">
         <v>564</v>
       </c>
+      <c r="K362" t="s">
+        <v>564</v>
+      </c>
       <c r="L362" t="s">
         <v>142</v>
       </c>
@@ -9233,6 +9348,9 @@
       <c r="G364" t="s">
         <v>564</v>
       </c>
+      <c r="K364" t="s">
+        <v>564</v>
+      </c>
       <c r="L364" t="s">
         <v>142</v>
       </c>
@@ -9304,11 +9422,14 @@
       <c r="E368" t="s">
         <v>564</v>
       </c>
+      <c r="K368" t="s">
+        <v>564</v>
+      </c>
       <c r="L368" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>3</v>
       </c>
@@ -9325,7 +9446,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>3</v>
       </c>
@@ -9342,7 +9463,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>3</v>
       </c>
@@ -9359,7 +9480,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>3</v>
       </c>
@@ -9375,11 +9496,14 @@
       <c r="G372" t="s">
         <v>564</v>
       </c>
+      <c r="K372" t="s">
+        <v>564</v>
+      </c>
       <c r="L372" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>3</v>
       </c>
@@ -9402,7 +9526,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>126</v>
       </c>
@@ -9419,7 +9543,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>126</v>
       </c>
@@ -9435,8 +9559,11 @@
       <c r="L375" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N375" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="376" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>126</v>
       </c>
@@ -9453,7 +9580,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>126</v>
       </c>
@@ -9470,7 +9597,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>126</v>
       </c>
@@ -9487,7 +9614,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B379" t="s">
         <v>525</v>
       </c>
@@ -9501,7 +9628,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B380" t="s">
         <v>525</v>
       </c>
@@ -9511,11 +9638,14 @@
       <c r="G380" t="s">
         <v>564</v>
       </c>
+      <c r="K380" t="s">
+        <v>564</v>
+      </c>
       <c r="M380" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B381" t="s">
         <v>525</v>
       </c>
@@ -9529,7 +9659,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B382" t="s">
         <v>525</v>
       </c>
@@ -9539,11 +9669,14 @@
       <c r="G382" t="s">
         <v>564</v>
       </c>
+      <c r="K382" t="s">
+        <v>564</v>
+      </c>
       <c r="M382" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B383" t="s">
         <v>555</v>
       </c>
@@ -9557,7 +9690,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B384" t="s">
         <v>555</v>
       </c>
@@ -9606,6 +9739,9 @@
       <c r="G387" t="s">
         <v>564</v>
       </c>
+      <c r="K387" t="s">
+        <v>564</v>
+      </c>
       <c r="M387" t="s">
         <v>577</v>
       </c>
@@ -9712,6 +9848,9 @@
       <c r="G395" t="s">
         <v>564</v>
       </c>
+      <c r="K395" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="396" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B396" t="s">
@@ -9746,9 +9885,12 @@
         <v>537</v>
       </c>
       <c r="D398" t="s">
-        <v>596</v>
+        <v>627</v>
       </c>
       <c r="G398" t="s">
+        <v>564</v>
+      </c>
+      <c r="K398" t="s">
         <v>564</v>
       </c>
       <c r="M398" t="s">
@@ -9763,7 +9905,7 @@
         <v>555</v>
       </c>
       <c r="D399" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G399" t="s">
         <v>564</v>
@@ -9780,7 +9922,7 @@
         <v>554</v>
       </c>
       <c r="D400" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G400" t="s">
         <v>564</v>
@@ -9797,7 +9939,7 @@
         <v>530</v>
       </c>
       <c r="D401" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G401" t="s">
         <v>564</v>
@@ -9808,10 +9950,10 @@
     </row>
     <row r="402" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B402" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D402" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G402" t="s">
         <v>564</v>
@@ -9825,7 +9967,7 @@
         <v>547</v>
       </c>
       <c r="D403" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G403" t="s">
         <v>564</v>
@@ -9839,7 +9981,7 @@
         <v>529</v>
       </c>
       <c r="D404" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G404" t="s">
         <v>564</v>
@@ -9847,10 +9989,10 @@
     </row>
     <row r="405" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B405" t="s">
+        <v>602</v>
+      </c>
+      <c r="D405" t="s">
         <v>603</v>
-      </c>
-      <c r="D405" t="s">
-        <v>604</v>
       </c>
       <c r="G405" t="s">
         <v>564</v>
@@ -9864,7 +10006,7 @@
         <v>555</v>
       </c>
       <c r="D406" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G406" t="s">
         <v>564</v>
@@ -9878,7 +10020,7 @@
         <v>529</v>
       </c>
       <c r="D407" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G407" t="s">
         <v>564</v>
@@ -9889,7 +10031,7 @@
         <v>529</v>
       </c>
       <c r="D408" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G408" t="s">
         <v>564</v>
@@ -9900,7 +10042,7 @@
         <v>554</v>
       </c>
       <c r="D409" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G409" t="s">
         <v>564</v>
@@ -9914,7 +10056,7 @@
         <v>547</v>
       </c>
       <c r="D410" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G410" t="s">
         <v>564</v>
@@ -9928,7 +10070,7 @@
         <v>555</v>
       </c>
       <c r="D411" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="G411" t="s">
         <v>564</v>
@@ -9942,7 +10084,7 @@
         <v>530</v>
       </c>
       <c r="D412" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="G412" t="s">
         <v>564</v>
@@ -9956,7 +10098,7 @@
         <v>530</v>
       </c>
       <c r="D413" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G413" t="s">
         <v>564</v>
@@ -9973,7 +10115,7 @@
         <v>554</v>
       </c>
       <c r="D414" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G414" t="s">
         <v>564</v>
@@ -9984,13 +10126,13 @@
         <v>559</v>
       </c>
       <c r="D415" t="s">
+        <v>614</v>
+      </c>
+      <c r="G415" t="s">
+        <v>564</v>
+      </c>
+      <c r="M415" t="s">
         <v>615</v>
-      </c>
-      <c r="G415" t="s">
-        <v>564</v>
-      </c>
-      <c r="M415" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="416" spans="2:13" x14ac:dyDescent="0.3">
@@ -9998,23 +10140,148 @@
         <v>519</v>
       </c>
       <c r="D416" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G416" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="417" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="417" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B417" t="s">
         <v>546</v>
       </c>
       <c r="D417" t="s">
+        <v>617</v>
+      </c>
+      <c r="G417" t="s">
+        <v>564</v>
+      </c>
+      <c r="M417" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="418" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B418" t="s">
+        <v>602</v>
+      </c>
+      <c r="C418" t="s">
+        <v>548</v>
+      </c>
+      <c r="D418" t="s">
         <v>618</v>
       </c>
-      <c r="G417" t="s">
-        <v>564</v>
-      </c>
-      <c r="M417" t="s">
+      <c r="K418" t="s">
+        <v>564</v>
+      </c>
+      <c r="N418" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="419" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B419" t="s">
+        <v>602</v>
+      </c>
+      <c r="D419" t="s">
+        <v>620</v>
+      </c>
+      <c r="G419" t="s">
+        <v>621</v>
+      </c>
+      <c r="K419" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="420" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B420" t="s">
+        <v>602</v>
+      </c>
+      <c r="C420" t="s">
+        <v>525</v>
+      </c>
+      <c r="D420" t="s">
+        <v>622</v>
+      </c>
+      <c r="K420" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="421" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B421" t="s">
+        <v>548</v>
+      </c>
+      <c r="D421" t="s">
+        <v>624</v>
+      </c>
+      <c r="K421" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="422" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B422" t="s">
+        <v>548</v>
+      </c>
+      <c r="D422" t="s">
+        <v>625</v>
+      </c>
+      <c r="K422" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="423" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B423" t="s">
+        <v>537</v>
+      </c>
+      <c r="D423" t="s">
+        <v>626</v>
+      </c>
+      <c r="K423" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="424" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B424" t="s">
+        <v>537</v>
+      </c>
+      <c r="D424" t="s">
+        <v>628</v>
+      </c>
+      <c r="K424" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="425" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B425" t="s">
+        <v>530</v>
+      </c>
+      <c r="D425" t="s">
+        <v>629</v>
+      </c>
+      <c r="K425" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="426" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B426" t="s">
+        <v>525</v>
+      </c>
+      <c r="D426" t="s">
+        <v>630</v>
+      </c>
+      <c r="K426" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="427" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B427" t="s">
+        <v>525</v>
+      </c>
+      <c r="D427" t="s">
+        <v>634</v>
+      </c>
+      <c r="K427" t="s">
+        <v>564</v>
+      </c>
+      <c r="N427" t="s">
         <v>577</v>
       </c>
     </row>

</xml_diff>